<commit_message>
add more explosion chem eqs
</commit_message>
<xml_diff>
--- a/templates/IO_notes.xlsx
+++ b/templates/IO_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="290" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="179">
   <si>
     <t>README_This file</t>
   </si>
@@ -26,7 +26,7 @@
     <t>This is a collection of notes about the names and order of some of the inputs and outputs</t>
   </si>
   <si>
-    <t>It also includes the appendix and notes section at the end of the excel outputs </t>
+    <t>It also includes the appendix and notes section at the end of the excel outputs</t>
   </si>
   <si>
     <t>Here is the Table of contents for this file</t>
@@ -53,7 +53,7 @@
     <t>The names off all the tested phenomenon for the model Mixing</t>
   </si>
   <si>
-    <t>PSI template </t>
+    <t>PSI template</t>
   </si>
   <si>
     <t>The template that is used to make a new safety info wkst which is then populated with the chemical names.</t>
@@ -278,7 +278,7 @@
     <t>mu</t>
   </si>
   <si>
-    <t>Viscosity air </t>
+    <t>Viscosity air</t>
   </si>
   <si>
     <t>muv</t>
@@ -441,6 +441,18 @@
   </si>
   <si>
     <t>dHexp</t>
+  </si>
+  <si>
+    <t>MinIgnitionEnergy</t>
+  </si>
+  <si>
+    <t>MIE</t>
+  </si>
+  <si>
+    <t>Impact Sensitivity</t>
+  </si>
+  <si>
+    <t>hdet50</t>
   </si>
   <si>
     <t>Irritation</t>
@@ -1060,10 +1072,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L52" activeCellId="0" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1442,71 +1454,71 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="M47" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="M47" s="0" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
+      <c r="M48" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M48" s="0" t="s">
+      <c r="M50" s="0" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M49" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M50" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="1" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>149</v>
+      </c>
       <c r="B52" s="1" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="M52" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M53" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="M54" s="0" t="s">
         <v>152</v>
@@ -1529,14 +1541,11 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="M57" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="M57" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,80 +1553,99 @@
         <v>159</v>
       </c>
       <c r="M58" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="1"/>
+      <c r="A59" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>160</v>
-      </c>
       <c r="B60" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="M60" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="M61" s="0" t="s">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
         <v>165</v>
       </c>
       <c r="M62" s="0" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="B63" s="1" t="s">
         <v>167</v>
       </c>
       <c r="M63" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M64" s="0" t="s">
-        <v>169</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
+      <c r="A65" s="0" t="s">
         <v>170</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="M65" s="0" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>172</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M67" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="M68" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="M69" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>